<commit_message>
feat: add confirmation dialog to input data batch menu
</commit_message>
<xml_diff>
--- a/AppTpp/bin/Release/net7.0-windows/temp/sampel import bactch data pegawai.xlsx
+++ b/AppTpp/bin/Release/net7.0-windows/temp/sampel import bactch data pegawai.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ekabu\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E71714EF-E2E0-4F38-B989-1364724A52FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F59DD52E-5C99-4A30-99FD-CC5131B5F394}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5AF2CE33-86B2-4676-A9C9-FBE112297AF1}"/>
   </bookViews>
@@ -114,12 +114,6 @@
     <t>040.201.0000142053</t>
   </si>
   <si>
-    <t>196512312007012112</t>
-  </si>
-  <si>
-    <t>NARMIN</t>
-  </si>
-  <si>
     <t>040.201.0000181342</t>
   </si>
   <si>
@@ -214,6 +208,12 @@
   </si>
   <si>
     <t>040.201.0000201947</t>
+  </si>
+  <si>
+    <t>196512421107012111</t>
+  </si>
+  <si>
+    <t>NARMINAL</t>
   </si>
 </sst>
 </file>
@@ -261,15 +261,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -582,13 +594,13 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.21875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.33203125" bestFit="1" customWidth="1"/>
@@ -602,7 +614,7 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
@@ -631,7 +643,7 @@
       <c r="A2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C2" t="s">
@@ -660,7 +672,7 @@
       <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C3" t="s">
@@ -689,7 +701,7 @@
       <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C4" t="s">
@@ -718,17 +730,17 @@
       <c r="A5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" t="s">
-        <v>26</v>
+      <c r="B5" s="2" t="s">
+        <v>58</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>59</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F5" t="s">
         <v>15</v>
@@ -747,17 +759,17 @@
       <c r="A6" t="s">
         <v>9</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" t="s">
         <v>32</v>
-      </c>
-      <c r="C6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" t="s">
-        <v>34</v>
       </c>
       <c r="F6" t="s">
         <v>13</v>
@@ -766,7 +778,7 @@
         <v>45865</v>
       </c>
       <c r="H6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I6" s="1">
         <v>3000000</v>
@@ -776,17 +788,17 @@
       <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" t="s">
         <v>35</v>
-      </c>
-      <c r="C7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7" t="s">
-        <v>37</v>
       </c>
       <c r="F7" t="s">
         <v>16</v>
@@ -795,7 +807,7 @@
         <v>60418</v>
       </c>
       <c r="H7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I7" s="1">
         <v>1000000</v>
@@ -805,17 +817,17 @@
       <c r="A8" t="s">
         <v>9</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" t="s">
         <v>39</v>
-      </c>
-      <c r="C8" t="s">
-        <v>40</v>
-      </c>
-      <c r="D8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" t="s">
-        <v>41</v>
       </c>
       <c r="F8" t="s">
         <v>15</v>
@@ -824,7 +836,7 @@
         <v>43878</v>
       </c>
       <c r="H8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I8" s="1">
         <v>2000000</v>
@@ -834,17 +846,17 @@
       <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" t="s">
         <v>42</v>
       </c>
-      <c r="C9" t="s">
+      <c r="E9" t="s">
         <v>43</v>
-      </c>
-      <c r="D9" t="s">
-        <v>44</v>
-      </c>
-      <c r="E9" t="s">
-        <v>45</v>
       </c>
       <c r="F9" t="s">
         <v>15</v>
@@ -853,7 +865,7 @@
         <v>46571</v>
       </c>
       <c r="H9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I9" s="1">
         <v>1000000</v>
@@ -863,26 +875,26 @@
       <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" t="s">
         <v>47</v>
       </c>
-      <c r="C10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D10" t="s">
-        <v>44</v>
-      </c>
-      <c r="E10" t="s">
-        <v>49</v>
-      </c>
       <c r="F10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G10">
         <v>76673</v>
       </c>
       <c r="H10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I10" s="1">
         <v>1000000</v>
@@ -892,17 +904,17 @@
       <c r="A11" t="s">
         <v>9</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" t="s">
         <v>50</v>
-      </c>
-      <c r="C11" t="s">
-        <v>51</v>
-      </c>
-      <c r="D11" t="s">
-        <v>44</v>
-      </c>
-      <c r="E11" t="s">
-        <v>52</v>
       </c>
       <c r="F11" t="s">
         <v>13</v>
@@ -911,7 +923,7 @@
         <v>43773</v>
       </c>
       <c r="H11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I11" s="1">
         <v>2000000</v>
@@ -921,17 +933,17 @@
       <c r="A12" t="s">
         <v>9</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" t="s">
         <v>53</v>
       </c>
-      <c r="C12" t="s">
+      <c r="E12" t="s">
         <v>54</v>
-      </c>
-      <c r="D12" t="s">
-        <v>55</v>
-      </c>
-      <c r="E12" t="s">
-        <v>56</v>
       </c>
       <c r="F12" t="s">
         <v>16</v>
@@ -940,7 +952,7 @@
         <v>64159</v>
       </c>
       <c r="H12" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I12" s="1">
         <v>1000000</v>
@@ -950,17 +962,17 @@
       <c r="A13" t="s">
         <v>9</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" t="s">
         <v>57</v>
-      </c>
-      <c r="C13" t="s">
-        <v>58</v>
-      </c>
-      <c r="D13" t="s">
-        <v>44</v>
-      </c>
-      <c r="E13" t="s">
-        <v>59</v>
       </c>
       <c r="F13" t="s">
         <v>11</v>
@@ -969,13 +981,16 @@
         <v>31608</v>
       </c>
       <c r="H13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I13" s="1">
         <v>2000000</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>